<commit_message>
Update RW Treegang's Mod Unit Catalogue (The Manh Files).xlsx
</commit_message>
<xml_diff>
--- a/RW Treegang's Mod Unit Catalogue (The Manh Files).xlsx
+++ b/RW Treegang's Mod Unit Catalogue (The Manh Files).xlsx
@@ -1,25 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Rusted Warfare\mods\units\test-mod\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7107E329-96C5-451B-8AC4-A24BD5EEA51C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-114" yWindow="-114" windowWidth="27602" windowHeight="14927" activeTab="1" xr2:uid="{C922FDEA-2633-42AC-944D-FFB76E45E754}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Fulgorian" sheetId="1" r:id="rId1"/>
     <sheet name="Oculian" sheetId="2" r:id="rId2"/>
     <sheet name="Dominion" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="185">
   <si>
     <t>T1</t>
   </si>
@@ -332,9 +326,6 @@
     <t>Fairy</t>
   </si>
   <si>
-    <t>Basic, Assault</t>
-  </si>
-  <si>
     <t>Dominion</t>
   </si>
   <si>
@@ -588,13 +579,19 @@
   </si>
   <si>
     <t>Cancer Mikanate</t>
+  </si>
+  <si>
+    <t>Harpy</t>
+  </si>
+  <si>
+    <t>Assault/Transport</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1184,7 +1181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
@@ -1422,66 +1419,6 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1506,6 +1443,66 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1557,9 +1554,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1629,7 +1627,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1681,7 +1679,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1875,21 +1873,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5CFCD23-8B28-4E9E-91D2-3A876416E6D1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T29"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="8.85546875" customWidth="1"/>
     <col min="4" max="4" width="8.85546875" customWidth="1"/>
@@ -1898,7 +1896,7 @@
     <col min="14" max="14" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="34.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="34.700000000000003" customHeight="1" thickBot="1">
       <c r="A1" s="35" t="s">
         <v>54</v>
       </c>
@@ -1922,7 +1920,7 @@
       <c r="S1" s="36"/>
       <c r="T1" s="37"/>
     </row>
-    <row r="2" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="14.45" customHeight="1">
       <c r="A2" s="44" t="s">
         <v>0</v>
       </c>
@@ -1950,7 +1948,7 @@
       <c r="S2" s="57"/>
       <c r="T2" s="58"/>
     </row>
-    <row r="3" spans="1:20" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="19.350000000000001" customHeight="1" thickBot="1">
       <c r="A3" s="47"/>
       <c r="B3" s="48"/>
       <c r="C3" s="48"/>
@@ -1972,7 +1970,7 @@
       <c r="S3" s="60"/>
       <c r="T3" s="61"/>
     </row>
-    <row r="4" spans="1:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="18" customHeight="1" thickBot="1">
       <c r="A4" s="38" t="s">
         <v>2</v>
       </c>
@@ -2012,7 +2010,7 @@
       </c>
       <c r="T4" s="34"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20">
       <c r="A5" s="16" t="s">
         <v>47</v>
       </c>
@@ -2070,7 +2068,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20">
       <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
@@ -2126,7 +2124,7 @@
       </c>
       <c r="T6" s="13"/>
     </row>
-    <row r="7" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="15" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>5</v>
       </c>
@@ -2180,7 +2178,7 @@
       <c r="S7" s="11"/>
       <c r="T7" s="6"/>
     </row>
-    <row r="8" spans="1:20" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="30">
       <c r="A8" s="11" t="s">
         <v>6</v>
       </c>
@@ -2230,7 +2228,7 @@
       <c r="S8" s="11"/>
       <c r="T8" s="6"/>
     </row>
-    <row r="9" spans="1:20" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="30">
       <c r="A9" s="11" t="s">
         <v>8</v>
       </c>
@@ -2280,7 +2278,7 @@
       <c r="S9" s="11"/>
       <c r="T9" s="6"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20">
       <c r="A10" s="11" t="s">
         <v>10</v>
       </c>
@@ -2322,7 +2320,7 @@
       <c r="S10" s="11"/>
       <c r="T10" s="6"/>
     </row>
-    <row r="11" spans="1:20" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="30">
       <c r="A11" s="11" t="s">
         <v>7</v>
       </c>
@@ -2352,7 +2350,7 @@
       <c r="S11" s="11"/>
       <c r="T11" s="6"/>
     </row>
-    <row r="12" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="15.75" thickBot="1">
       <c r="A12" s="19" t="s">
         <v>9</v>
       </c>
@@ -2382,13 +2380,13 @@
       <c r="S12" s="19"/>
       <c r="T12" s="20"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20">
       <c r="A14" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="7:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="14.45" customHeight="1"/>
+    <row r="20" spans="7:20" ht="14.45" customHeight="1">
       <c r="G20" s="12"/>
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
@@ -2400,7 +2398,7 @@
       <c r="S20" s="7"/>
       <c r="T20" s="7"/>
     </row>
-    <row r="21" spans="7:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:20" ht="14.45" customHeight="1">
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
@@ -2411,7 +2409,7 @@
       <c r="S21" s="7"/>
       <c r="T21" s="7"/>
     </row>
-    <row r="22" spans="7:20" ht="16.399999999999999" x14ac:dyDescent="0.25">
+    <row r="22" spans="7:20" ht="15.75">
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8"/>
@@ -2422,10 +2420,10 @@
       <c r="S22" s="8"/>
       <c r="T22" s="8"/>
     </row>
-    <row r="23" spans="7:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:20">
       <c r="T23" s="9"/>
     </row>
-    <row r="29" spans="7:20" ht="18.55" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="7:20" ht="18.600000000000001" customHeight="1"/>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="O4:P4"/>
@@ -2448,14 +2446,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CE861A1-FC41-4124-9311-B732643B6141}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" customWidth="1"/>
@@ -2472,7 +2470,7 @@
     <col min="20" max="20" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="36.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="36" thickBot="1">
       <c r="A1" s="64" t="s">
         <v>68</v>
       </c>
@@ -2496,7 +2494,7 @@
       <c r="S1" s="65"/>
       <c r="T1" s="66"/>
     </row>
-    <row r="2" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="14.45" customHeight="1">
       <c r="A2" s="67" t="s">
         <v>0</v>
       </c>
@@ -2524,7 +2522,7 @@
       <c r="S2" s="80"/>
       <c r="T2" s="81"/>
     </row>
-    <row r="3" spans="1:20" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="19.350000000000001" customHeight="1" thickBot="1">
       <c r="A3" s="70"/>
       <c r="B3" s="71"/>
       <c r="C3" s="71"/>
@@ -2546,7 +2544,7 @@
       <c r="S3" s="83"/>
       <c r="T3" s="84"/>
     </row>
-    <row r="4" spans="1:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="18" customHeight="1" thickBot="1">
       <c r="A4" s="38" t="s">
         <v>2</v>
       </c>
@@ -2586,7 +2584,7 @@
       </c>
       <c r="T4" s="63"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20">
       <c r="A5" s="16" t="s">
         <v>47</v>
       </c>
@@ -2642,7 +2640,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20">
       <c r="A6" s="11" t="s">
         <v>69</v>
       </c>
@@ -2672,7 +2670,7 @@
         <v>87</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="L6" s="11" t="s">
         <v>90</v>
@@ -2682,13 +2680,13 @@
       </c>
       <c r="N6" s="12"/>
       <c r="O6" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="P6" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q6" s="11" t="s">
         <v>177</v>
-      </c>
-      <c r="Q6" s="11" t="s">
-        <v>178</v>
       </c>
       <c r="R6" s="13" t="s">
         <v>48</v>
@@ -2700,88 +2698,88 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="27.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="27.6" customHeight="1">
       <c r="A7" s="11" t="s">
         <v>70</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C7" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>162</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>80</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G7" s="12"/>
       <c r="H7" s="10" t="s">
         <v>84</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K7" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="L7" s="11" t="s">
         <v>91</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="N7" s="12"/>
       <c r="O7" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="P7" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="P7" s="6" t="s">
-        <v>176</v>
-      </c>
       <c r="Q7" s="11" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="S7" s="11"/>
       <c r="T7" s="6"/>
     </row>
-    <row r="8" spans="1:20" ht="42.8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="30">
       <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C8" s="11" t="s">
         <v>76</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E8" s="11" t="s">
         <v>81</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G8" s="12"/>
       <c r="H8" s="10" t="s">
         <v>85</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K8" s="6" t="s">
         <v>12</v>
@@ -2796,26 +2794,26 @@
       <c r="O8" s="11"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="11" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="S8" s="11"/>
       <c r="T8" s="6"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20">
       <c r="A9" s="11" t="s">
         <v>72</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C9" s="11" t="s">
         <v>77</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="6"/>
@@ -2836,26 +2834,26 @@
         <v>93</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="N9" s="12"/>
       <c r="O9" s="11"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="11" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="R9" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="S9" s="11"/>
       <c r="T9" s="6"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20">
       <c r="A10" s="11" t="s">
         <v>73</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>78</v>
@@ -2872,19 +2870,19 @@
         <v>89</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="L10" s="11" t="s">
         <v>94</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N10" s="12"/>
       <c r="O10" s="11"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="11" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="R10" s="6" t="s">
         <v>55</v>
@@ -2892,7 +2890,7 @@
       <c r="S10" s="11"/>
       <c r="T10" s="6"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20">
       <c r="A11" s="11" t="s">
         <v>74</v>
       </c>
@@ -2912,19 +2910,19 @@
         <v>95</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="N11" s="12"/>
       <c r="O11" s="10"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="11" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="R11" s="6"/>
       <c r="S11" s="11"/>
       <c r="T11" s="6"/>
     </row>
-    <row r="12" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="15.75" thickBot="1">
       <c r="A12" s="19"/>
       <c r="B12" s="20"/>
       <c r="C12" s="19"/>
@@ -2940,7 +2938,7 @@
         <v>96</v>
       </c>
       <c r="M12" s="20" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="N12" s="12"/>
       <c r="O12" s="21"/>
@@ -2950,10 +2948,10 @@
       <c r="S12" s="19"/>
       <c r="T12" s="20"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20">
       <c r="A15" s="24"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20">
       <c r="A16" s="24"/>
     </row>
   </sheetData>
@@ -2977,75 +2975,76 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE9D55B1-5E12-47E2-9276-8FA43FC187EC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF16"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AC34" sqref="AC34"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.140625" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
     <col min="7" max="7" width="8.5703125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
     <col min="9" max="9" width="10.28515625" customWidth="1"/>
     <col min="10" max="10" width="8.5703125" customWidth="1"/>
     <col min="11" max="11" width="4.7109375" customWidth="1"/>
     <col min="12" max="12" width="10.28515625" customWidth="1"/>
-    <col min="13" max="13" width="8" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" customWidth="1"/>
     <col min="14" max="14" width="11.42578125" customWidth="1"/>
     <col min="15" max="15" width="9.7109375" customWidth="1"/>
     <col min="16" max="17" width="8.85546875" customWidth="1"/>
     <col min="18" max="18" width="9.28515625" customWidth="1"/>
+    <col min="19" max="19" width="17.85546875" customWidth="1"/>
     <col min="20" max="20" width="11.5703125" customWidth="1"/>
     <col min="21" max="21" width="8.5703125" customWidth="1"/>
     <col min="22" max="22" width="4.85546875" customWidth="1"/>
     <col min="31" max="31" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="34.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="85" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-      <c r="L1" s="86"/>
-      <c r="M1" s="86"/>
-      <c r="N1" s="86"/>
-      <c r="O1" s="86"/>
-      <c r="P1" s="86"/>
-      <c r="Q1" s="86"/>
-      <c r="R1" s="86"/>
-      <c r="S1" s="86"/>
-      <c r="T1" s="86"/>
-      <c r="U1" s="86"/>
-      <c r="V1" s="86"/>
-      <c r="W1" s="86"/>
-      <c r="X1" s="86"/>
-      <c r="Y1" s="86"/>
-      <c r="Z1" s="86"/>
-      <c r="AA1" s="86"/>
-      <c r="AB1" s="86"/>
-      <c r="AC1" s="86"/>
-      <c r="AD1" s="86"/>
-      <c r="AE1" s="86"/>
-      <c r="AF1" s="86"/>
-    </row>
-    <row r="2" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" ht="34.700000000000003" customHeight="1" thickBot="1">
+      <c r="A1" s="105" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="106"/>
+      <c r="C1" s="106"/>
+      <c r="D1" s="106"/>
+      <c r="E1" s="106"/>
+      <c r="F1" s="106"/>
+      <c r="G1" s="106"/>
+      <c r="H1" s="106"/>
+      <c r="I1" s="106"/>
+      <c r="J1" s="106"/>
+      <c r="K1" s="106"/>
+      <c r="L1" s="106"/>
+      <c r="M1" s="106"/>
+      <c r="N1" s="106"/>
+      <c r="O1" s="106"/>
+      <c r="P1" s="106"/>
+      <c r="Q1" s="106"/>
+      <c r="R1" s="106"/>
+      <c r="S1" s="106"/>
+      <c r="T1" s="106"/>
+      <c r="U1" s="106"/>
+      <c r="V1" s="106"/>
+      <c r="W1" s="106"/>
+      <c r="X1" s="106"/>
+      <c r="Y1" s="106"/>
+      <c r="Z1" s="106"/>
+      <c r="AA1" s="106"/>
+      <c r="AB1" s="106"/>
+      <c r="AC1" s="106"/>
+      <c r="AD1" s="106"/>
+      <c r="AE1" s="106"/>
+      <c r="AF1" s="106"/>
+    </row>
+    <row r="2" spans="1:32" ht="15" customHeight="1">
       <c r="A2" s="113" t="s">
         <v>0</v>
       </c>
@@ -3070,20 +3069,20 @@
       <c r="S2" s="120"/>
       <c r="T2" s="120"/>
       <c r="U2" s="121"/>
-      <c r="W2" s="87" t="s">
+      <c r="W2" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="X2" s="88"/>
-      <c r="Y2" s="88"/>
-      <c r="Z2" s="88"/>
-      <c r="AA2" s="88"/>
-      <c r="AB2" s="88"/>
-      <c r="AC2" s="88"/>
-      <c r="AD2" s="88"/>
-      <c r="AE2" s="88"/>
-      <c r="AF2" s="89"/>
-    </row>
-    <row r="3" spans="1:32" ht="19.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="X2" s="108"/>
+      <c r="Y2" s="108"/>
+      <c r="Z2" s="108"/>
+      <c r="AA2" s="108"/>
+      <c r="AB2" s="108"/>
+      <c r="AC2" s="108"/>
+      <c r="AD2" s="108"/>
+      <c r="AE2" s="108"/>
+      <c r="AF2" s="109"/>
+    </row>
+    <row r="3" spans="1:32" ht="19.350000000000001" customHeight="1" thickBot="1">
       <c r="A3" s="116"/>
       <c r="B3" s="117"/>
       <c r="C3" s="117"/>
@@ -3104,18 +3103,18 @@
       <c r="S3" s="123"/>
       <c r="T3" s="123"/>
       <c r="U3" s="124"/>
-      <c r="W3" s="90"/>
-      <c r="X3" s="91"/>
-      <c r="Y3" s="91"/>
-      <c r="Z3" s="91"/>
-      <c r="AA3" s="91"/>
-      <c r="AB3" s="91"/>
-      <c r="AC3" s="91"/>
-      <c r="AD3" s="91"/>
-      <c r="AE3" s="91"/>
-      <c r="AF3" s="92"/>
-    </row>
-    <row r="4" spans="1:32" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W3" s="110"/>
+      <c r="X3" s="111"/>
+      <c r="Y3" s="111"/>
+      <c r="Z3" s="111"/>
+      <c r="AA3" s="111"/>
+      <c r="AB3" s="111"/>
+      <c r="AC3" s="111"/>
+      <c r="AD3" s="111"/>
+      <c r="AE3" s="111"/>
+      <c r="AF3" s="112"/>
+    </row>
+    <row r="4" spans="1:32" ht="18" customHeight="1">
       <c r="A4" s="93" t="s">
         <v>2</v>
       </c>
@@ -3128,10 +3127,10 @@
         <v>1</v>
       </c>
       <c r="H4" s="100"/>
-      <c r="I4" s="105" t="s">
+      <c r="I4" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="106"/>
+      <c r="J4" s="86"/>
       <c r="L4" s="93" t="s">
         <v>2</v>
       </c>
@@ -3144,10 +3143,10 @@
         <v>1</v>
       </c>
       <c r="S4" s="100"/>
-      <c r="T4" s="105" t="s">
+      <c r="T4" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="U4" s="106"/>
+      <c r="U4" s="86"/>
       <c r="W4" s="93" t="s">
         <v>2</v>
       </c>
@@ -3160,12 +3159,12 @@
         <v>1</v>
       </c>
       <c r="AD4" s="100"/>
-      <c r="AE4" s="105" t="s">
+      <c r="AE4" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="AF4" s="106"/>
-    </row>
-    <row r="5" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AF4" s="86"/>
+    </row>
+    <row r="5" spans="1:32" ht="15.75" thickBot="1">
       <c r="A5" s="96"/>
       <c r="B5" s="97"/>
       <c r="C5" s="97"/>
@@ -3174,8 +3173,8 @@
       <c r="F5" s="98"/>
       <c r="G5" s="101"/>
       <c r="H5" s="102"/>
-      <c r="I5" s="107"/>
-      <c r="J5" s="108"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="88"/>
       <c r="L5" s="96"/>
       <c r="M5" s="97"/>
       <c r="N5" s="97"/>
@@ -3184,8 +3183,8 @@
       <c r="Q5" s="126"/>
       <c r="R5" s="101"/>
       <c r="S5" s="102"/>
-      <c r="T5" s="107"/>
-      <c r="U5" s="108"/>
+      <c r="T5" s="87"/>
+      <c r="U5" s="88"/>
       <c r="W5" s="96"/>
       <c r="X5" s="97"/>
       <c r="Y5" s="97"/>
@@ -3194,60 +3193,60 @@
       <c r="AB5" s="98"/>
       <c r="AC5" s="101"/>
       <c r="AD5" s="102"/>
-      <c r="AE5" s="107"/>
-      <c r="AF5" s="108"/>
-    </row>
-    <row r="6" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="111" t="s">
+      <c r="AE5" s="87"/>
+      <c r="AF5" s="88"/>
+    </row>
+    <row r="6" spans="1:32" ht="15.75" thickBot="1">
+      <c r="A6" s="91" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="92"/>
+      <c r="C6" s="91" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="112"/>
-      <c r="C6" s="111" t="s">
+      <c r="D6" s="92"/>
+      <c r="E6" s="91" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="112"/>
-      <c r="E6" s="111" t="s">
-        <v>102</v>
-      </c>
-      <c r="F6" s="112"/>
+      <c r="F6" s="92"/>
       <c r="G6" s="103"/>
       <c r="H6" s="104"/>
-      <c r="I6" s="109"/>
-      <c r="J6" s="110"/>
-      <c r="L6" s="111" t="s">
+      <c r="I6" s="89"/>
+      <c r="J6" s="90"/>
+      <c r="L6" s="91" t="s">
+        <v>99</v>
+      </c>
+      <c r="M6" s="92"/>
+      <c r="N6" s="127" t="s">
         <v>100</v>
-      </c>
-      <c r="M6" s="112"/>
-      <c r="N6" s="127" t="s">
-        <v>101</v>
       </c>
       <c r="O6" s="127"/>
       <c r="P6" s="128" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="Q6" s="129"/>
       <c r="R6" s="103"/>
       <c r="S6" s="104"/>
-      <c r="T6" s="109"/>
-      <c r="U6" s="110"/>
-      <c r="W6" s="111" t="s">
+      <c r="T6" s="89"/>
+      <c r="U6" s="90"/>
+      <c r="W6" s="91" t="s">
+        <v>99</v>
+      </c>
+      <c r="X6" s="92"/>
+      <c r="Y6" s="91" t="s">
         <v>100</v>
       </c>
-      <c r="X6" s="112"/>
-      <c r="Y6" s="111" t="s">
+      <c r="Z6" s="92"/>
+      <c r="AA6" s="91" t="s">
         <v>101</v>
       </c>
-      <c r="Z6" s="112"/>
-      <c r="AA6" s="111" t="s">
-        <v>102</v>
-      </c>
-      <c r="AB6" s="112"/>
+      <c r="AB6" s="92"/>
       <c r="AC6" s="103"/>
       <c r="AD6" s="104"/>
-      <c r="AE6" s="109"/>
-      <c r="AF6" s="110"/>
-    </row>
-    <row r="7" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE6" s="89"/>
+      <c r="AF6" s="90"/>
+    </row>
+    <row r="7" spans="1:32" ht="15.75" thickBot="1">
       <c r="A7" s="25" t="s">
         <v>47</v>
       </c>
@@ -3339,9 +3338,9 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:32" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" ht="30">
       <c r="A8" s="10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>51</v>
@@ -3353,49 +3352,49 @@
         <v>9</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>53</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>52</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>48</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O8" s="28" t="s">
         <v>9</v>
       </c>
       <c r="P8" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q8" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="R8" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="Q8" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="R8" s="10" t="s">
-        <v>147</v>
-      </c>
       <c r="S8" s="13" t="s">
-        <v>58</v>
+        <v>176</v>
       </c>
       <c r="T8" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="U8" s="13" t="s">
         <v>48</v>
@@ -3417,51 +3416,51 @@
       </c>
       <c r="AD8" s="6"/>
       <c r="AE8" s="10" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="AF8" s="6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" ht="15" customHeight="1">
       <c r="A9" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>48</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>48</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>48</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H9" s="6" t="s">
-        <v>58</v>
+        <v>176</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J9" s="6" t="s">
         <v>62</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>58</v>
+        <v>157</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O9" s="28" t="s">
         <v>48</v>
@@ -3469,13 +3468,13 @@
       <c r="P9" s="10"/>
       <c r="Q9" s="28"/>
       <c r="R9" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="S9" s="6" t="s">
         <v>52</v>
       </c>
       <c r="T9" s="10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="U9" s="6" t="s">
         <v>62</v>
@@ -3489,39 +3488,39 @@
       <c r="AC9" s="10"/>
       <c r="AD9" s="6"/>
       <c r="AE9" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="AF9" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:32" ht="28.2" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" ht="28.15" customHeight="1">
       <c r="A10" s="10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>62</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>62</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>12</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="J10" s="6" t="s">
         <v>57</v>
@@ -3529,21 +3528,21 @@
       <c r="L10" s="10"/>
       <c r="M10" s="6"/>
       <c r="N10" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="O10" s="28" t="s">
-        <v>98</v>
+        <v>176</v>
       </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="28"/>
       <c r="R10" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="S10" s="6" t="s">
         <v>12</v>
       </c>
       <c r="T10" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="U10" s="6" t="s">
         <v>57</v>
@@ -3559,33 +3558,33 @@
       <c r="AE10" s="10"/>
       <c r="AF10" s="6"/>
     </row>
-    <row r="11" spans="1:32" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" ht="30">
       <c r="A11" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>57</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>50</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>50</v>
+        <v>157</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I11" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="J11" s="6" t="s">
         <v>61</v>
@@ -3593,17 +3592,21 @@
       <c r="L11" s="10"/>
       <c r="M11" s="6"/>
       <c r="N11" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="O11" s="28" t="s">
         <v>58</v>
       </c>
       <c r="P11" s="10"/>
       <c r="Q11" s="28"/>
-      <c r="R11" s="10"/>
-      <c r="S11" s="2"/>
+      <c r="R11" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="S11" s="130" t="s">
+        <v>184</v>
+      </c>
       <c r="T11" s="10" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="U11" s="6" t="s">
         <v>61</v>
@@ -3619,27 +3622,27 @@
       <c r="AE11" s="10"/>
       <c r="AF11" s="6"/>
     </row>
-    <row r="12" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" ht="15" customHeight="1">
       <c r="A12" s="10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>58</v>
+        <v>157</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>57</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>62</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>51</v>
@@ -3649,7 +3652,7 @@
       <c r="L12" s="10"/>
       <c r="M12" s="6"/>
       <c r="N12" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O12" s="28" t="s">
         <v>61</v>
@@ -3671,37 +3674,37 @@
       <c r="AE12" s="10"/>
       <c r="AF12" s="6"/>
     </row>
-    <row r="13" spans="1:32" ht="28.55" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32">
       <c r="A13" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>48</v>
+        <v>176</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>61</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>61</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="6"/>
       <c r="L13" s="10"/>
       <c r="M13" s="6"/>
       <c r="N13" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O13" s="28" t="s">
         <v>62</v>
@@ -3723,21 +3726,21 @@
       <c r="AE13" s="10"/>
       <c r="AF13" s="6"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32">
       <c r="A14" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>61</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>50</v>
@@ -3749,7 +3752,7 @@
       <c r="L14" s="10"/>
       <c r="M14" s="6"/>
       <c r="N14" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O14" s="28" t="s">
         <v>50</v>
@@ -3771,20 +3774,20 @@
       <c r="AE14" s="10"/>
       <c r="AF14" s="6"/>
     </row>
-    <row r="15" spans="1:32" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" ht="15" customHeight="1" thickBot="1">
       <c r="A15" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="20" t="s">
         <v>110</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>111</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="3"/>
       <c r="E15" s="21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F15" s="20" t="s">
-        <v>58</v>
+        <v>176</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="3"/>
@@ -3793,10 +3796,10 @@
       <c r="L15" s="10"/>
       <c r="M15" s="6"/>
       <c r="N15" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="O15" t="s">
         <v>143</v>
-      </c>
-      <c r="O15" t="s">
-        <v>144</v>
       </c>
       <c r="P15" s="10"/>
       <c r="Q15" s="28"/>
@@ -3815,14 +3818,14 @@
       <c r="AE15" s="5"/>
       <c r="AF15" s="3"/>
     </row>
-    <row r="16" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" ht="15.75" thickBot="1">
       <c r="L16" s="5"/>
       <c r="M16" s="3"/>
       <c r="N16" s="29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P16" s="5"/>
       <c r="Q16" s="31"/>
@@ -3833,12 +3836,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="I4:J6"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="A4:F5"/>
-    <mergeCell ref="G4:H6"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="W2:AF3"/>
     <mergeCell ref="W4:AB5"/>
@@ -3855,7 +3852,14 @@
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="I4:J6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A4:F5"/>
+    <mergeCell ref="G4:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
buffed testudo and some infantry, added Faust unit, made harpy missiles more reliable.
</commit_message>
<xml_diff>
--- a/RW Treegang's Mod Unit Catalogue (The Manh Files).xlsx
+++ b/RW Treegang's Mod Unit Catalogue (The Manh Files).xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="188">
   <si>
     <t>T1</t>
   </si>
@@ -591,6 +591,9 @@
   </si>
   <si>
     <t>Ungutem</t>
+  </si>
+  <si>
+    <t>Faust</t>
   </si>
 </sst>
 </file>
@@ -1426,66 +1429,6 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1509,6 +1452,66 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1879,7 +1882,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2984,8 +2987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3006,7 +3009,7 @@
     <col min="14" max="14" width="11.42578125" customWidth="1"/>
     <col min="15" max="15" width="9.7109375" customWidth="1"/>
     <col min="16" max="16" width="11.28515625" customWidth="1"/>
-    <col min="17" max="17" width="8.85546875" customWidth="1"/>
+    <col min="17" max="17" width="10.85546875" customWidth="1"/>
     <col min="18" max="18" width="9.28515625" customWidth="1"/>
     <col min="19" max="19" width="17.85546875" customWidth="1"/>
     <col min="20" max="20" width="11.5703125" customWidth="1"/>
@@ -3016,40 +3019,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="34.700000000000003" customHeight="1" thickBot="1">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="106" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="87"/>
-      <c r="R1" s="87"/>
-      <c r="S1" s="87"/>
-      <c r="T1" s="87"/>
-      <c r="U1" s="87"/>
-      <c r="V1" s="87"/>
-      <c r="W1" s="87"/>
-      <c r="X1" s="87"/>
-      <c r="Y1" s="87"/>
-      <c r="Z1" s="87"/>
-      <c r="AA1" s="87"/>
-      <c r="AB1" s="87"/>
-      <c r="AC1" s="87"/>
-      <c r="AD1" s="87"/>
-      <c r="AE1" s="87"/>
-      <c r="AF1" s="87"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
+      <c r="Q1" s="107"/>
+      <c r="R1" s="107"/>
+      <c r="S1" s="107"/>
+      <c r="T1" s="107"/>
+      <c r="U1" s="107"/>
+      <c r="V1" s="107"/>
+      <c r="W1" s="107"/>
+      <c r="X1" s="107"/>
+      <c r="Y1" s="107"/>
+      <c r="Z1" s="107"/>
+      <c r="AA1" s="107"/>
+      <c r="AB1" s="107"/>
+      <c r="AC1" s="107"/>
+      <c r="AD1" s="107"/>
+      <c r="AE1" s="107"/>
+      <c r="AF1" s="107"/>
     </row>
     <row r="2" spans="1:32" ht="15" customHeight="1">
       <c r="A2" s="114" t="s">
@@ -3076,18 +3079,18 @@
       <c r="S2" s="121"/>
       <c r="T2" s="121"/>
       <c r="U2" s="122"/>
-      <c r="W2" s="88" t="s">
+      <c r="W2" s="108" t="s">
         <v>18</v>
       </c>
-      <c r="X2" s="89"/>
-      <c r="Y2" s="89"/>
-      <c r="Z2" s="89"/>
-      <c r="AA2" s="89"/>
-      <c r="AB2" s="89"/>
-      <c r="AC2" s="89"/>
-      <c r="AD2" s="89"/>
-      <c r="AE2" s="89"/>
-      <c r="AF2" s="90"/>
+      <c r="X2" s="109"/>
+      <c r="Y2" s="109"/>
+      <c r="Z2" s="109"/>
+      <c r="AA2" s="109"/>
+      <c r="AB2" s="109"/>
+      <c r="AC2" s="109"/>
+      <c r="AD2" s="109"/>
+      <c r="AE2" s="109"/>
+      <c r="AF2" s="110"/>
     </row>
     <row r="3" spans="1:32" ht="19.350000000000001" customHeight="1" thickBot="1">
       <c r="A3" s="117"/>
@@ -3110,16 +3113,16 @@
       <c r="S3" s="124"/>
       <c r="T3" s="124"/>
       <c r="U3" s="125"/>
-      <c r="W3" s="91"/>
-      <c r="X3" s="92"/>
-      <c r="Y3" s="92"/>
-      <c r="Z3" s="92"/>
-      <c r="AA3" s="92"/>
-      <c r="AB3" s="92"/>
-      <c r="AC3" s="92"/>
-      <c r="AD3" s="92"/>
-      <c r="AE3" s="92"/>
-      <c r="AF3" s="93"/>
+      <c r="W3" s="111"/>
+      <c r="X3" s="112"/>
+      <c r="Y3" s="112"/>
+      <c r="Z3" s="112"/>
+      <c r="AA3" s="112"/>
+      <c r="AB3" s="112"/>
+      <c r="AC3" s="112"/>
+      <c r="AD3" s="112"/>
+      <c r="AE3" s="112"/>
+      <c r="AF3" s="113"/>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1">
       <c r="A4" s="94" t="s">
@@ -3134,10 +3137,10 @@
         <v>1</v>
       </c>
       <c r="H4" s="101"/>
-      <c r="I4" s="106" t="s">
+      <c r="I4" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="107"/>
+      <c r="J4" s="87"/>
       <c r="L4" s="94" t="s">
         <v>2</v>
       </c>
@@ -3150,10 +3153,10 @@
         <v>1</v>
       </c>
       <c r="S4" s="101"/>
-      <c r="T4" s="106" t="s">
+      <c r="T4" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="U4" s="107"/>
+      <c r="U4" s="87"/>
       <c r="W4" s="94" t="s">
         <v>2</v>
       </c>
@@ -3166,10 +3169,10 @@
         <v>1</v>
       </c>
       <c r="AD4" s="101"/>
-      <c r="AE4" s="106" t="s">
+      <c r="AE4" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="AF4" s="107"/>
+      <c r="AF4" s="87"/>
     </row>
     <row r="5" spans="1:32" ht="15.75" thickBot="1">
       <c r="A5" s="97"/>
@@ -3180,8 +3183,8 @@
       <c r="F5" s="99"/>
       <c r="G5" s="102"/>
       <c r="H5" s="103"/>
-      <c r="I5" s="108"/>
-      <c r="J5" s="109"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="89"/>
       <c r="L5" s="97"/>
       <c r="M5" s="98"/>
       <c r="N5" s="98"/>
@@ -3190,8 +3193,8 @@
       <c r="Q5" s="127"/>
       <c r="R5" s="102"/>
       <c r="S5" s="103"/>
-      <c r="T5" s="108"/>
-      <c r="U5" s="109"/>
+      <c r="T5" s="88"/>
+      <c r="U5" s="89"/>
       <c r="W5" s="97"/>
       <c r="X5" s="98"/>
       <c r="Y5" s="98"/>
@@ -3200,30 +3203,30 @@
       <c r="AB5" s="99"/>
       <c r="AC5" s="102"/>
       <c r="AD5" s="103"/>
-      <c r="AE5" s="108"/>
-      <c r="AF5" s="109"/>
+      <c r="AE5" s="88"/>
+      <c r="AF5" s="89"/>
     </row>
     <row r="6" spans="1:32" ht="15.75" thickBot="1">
-      <c r="A6" s="112" t="s">
+      <c r="A6" s="92" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="113"/>
-      <c r="C6" s="112" t="s">
+      <c r="B6" s="93"/>
+      <c r="C6" s="92" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="113"/>
-      <c r="E6" s="112" t="s">
+      <c r="D6" s="93"/>
+      <c r="E6" s="92" t="s">
         <v>101</v>
       </c>
-      <c r="F6" s="113"/>
+      <c r="F6" s="93"/>
       <c r="G6" s="104"/>
       <c r="H6" s="105"/>
-      <c r="I6" s="110"/>
-      <c r="J6" s="111"/>
-      <c r="L6" s="112" t="s">
+      <c r="I6" s="90"/>
+      <c r="J6" s="91"/>
+      <c r="L6" s="92" t="s">
         <v>99</v>
       </c>
-      <c r="M6" s="113"/>
+      <c r="M6" s="93"/>
       <c r="N6" s="128" t="s">
         <v>100</v>
       </c>
@@ -3234,24 +3237,24 @@
       <c r="Q6" s="130"/>
       <c r="R6" s="104"/>
       <c r="S6" s="105"/>
-      <c r="T6" s="110"/>
-      <c r="U6" s="111"/>
-      <c r="W6" s="112" t="s">
+      <c r="T6" s="90"/>
+      <c r="U6" s="91"/>
+      <c r="W6" s="92" t="s">
         <v>99</v>
       </c>
-      <c r="X6" s="113"/>
-      <c r="Y6" s="112" t="s">
+      <c r="X6" s="93"/>
+      <c r="Y6" s="92" t="s">
         <v>100</v>
       </c>
-      <c r="Z6" s="113"/>
-      <c r="AA6" s="112" t="s">
+      <c r="Z6" s="93"/>
+      <c r="AA6" s="92" t="s">
         <v>101</v>
       </c>
-      <c r="AB6" s="113"/>
+      <c r="AB6" s="93"/>
       <c r="AC6" s="104"/>
       <c r="AD6" s="105"/>
-      <c r="AE6" s="110"/>
-      <c r="AF6" s="111"/>
+      <c r="AE6" s="90"/>
+      <c r="AF6" s="91"/>
     </row>
     <row r="7" spans="1:32" ht="15.75" thickBot="1">
       <c r="A7" s="25" t="s">
@@ -3612,8 +3615,12 @@
       <c r="O11" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="P11" s="10"/>
-      <c r="Q11" s="28"/>
+      <c r="P11" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q11" s="28" t="s">
+        <v>157</v>
+      </c>
       <c r="R11" s="10" t="s">
         <v>183</v>
       </c>
@@ -3851,12 +3858,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="I4:J6"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="A4:F5"/>
-    <mergeCell ref="G4:H6"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="W2:AF3"/>
     <mergeCell ref="W4:AB5"/>
@@ -3873,6 +3874,12 @@
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="I4:J6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A4:F5"/>
+    <mergeCell ref="G4:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fixed thumbnail, added units to sheet
</commit_message>
<xml_diff>
--- a/RW Treegang's Mod Unit Catalogue (The Manh Files).xlsx
+++ b/RW Treegang's Mod Unit Catalogue (The Manh Files).xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="193">
   <si>
     <t>T1</t>
   </si>
@@ -594,6 +594,21 @@
   </si>
   <si>
     <t>Faust</t>
+  </si>
+  <si>
+    <t>Field gun</t>
+  </si>
+  <si>
+    <t>Skirmisher/Artillery</t>
+  </si>
+  <si>
+    <t>Schockwelle</t>
+  </si>
+  <si>
+    <t>A-swarm</t>
+  </si>
+  <si>
+    <t>Klatsche</t>
   </si>
 </sst>
 </file>
@@ -1429,6 +1444,66 @@
     <xf numFmtId="0" fontId="2" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1452,66 +1527,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1882,7 +1897,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2987,8 +3002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AF16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3008,8 +3023,8 @@
     <col min="13" max="13" width="11.28515625" customWidth="1"/>
     <col min="14" max="14" width="11.42578125" customWidth="1"/>
     <col min="15" max="15" width="9.7109375" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" customWidth="1"/>
-    <col min="17" max="17" width="10.85546875" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" customWidth="1"/>
+    <col min="17" max="17" width="18.42578125" customWidth="1"/>
     <col min="18" max="18" width="9.28515625" customWidth="1"/>
     <col min="19" max="19" width="17.85546875" customWidth="1"/>
     <col min="20" max="20" width="11.5703125" customWidth="1"/>
@@ -3019,40 +3034,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="34.700000000000003" customHeight="1" thickBot="1">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="86" t="s">
         <v>98</v>
       </c>
-      <c r="B1" s="107"/>
-      <c r="C1" s="107"/>
-      <c r="D1" s="107"/>
-      <c r="E1" s="107"/>
-      <c r="F1" s="107"/>
-      <c r="G1" s="107"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="107"/>
-      <c r="J1" s="107"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
-      <c r="M1" s="107"/>
-      <c r="N1" s="107"/>
-      <c r="O1" s="107"/>
-      <c r="P1" s="107"/>
-      <c r="Q1" s="107"/>
-      <c r="R1" s="107"/>
-      <c r="S1" s="107"/>
-      <c r="T1" s="107"/>
-      <c r="U1" s="107"/>
-      <c r="V1" s="107"/>
-      <c r="W1" s="107"/>
-      <c r="X1" s="107"/>
-      <c r="Y1" s="107"/>
-      <c r="Z1" s="107"/>
-      <c r="AA1" s="107"/>
-      <c r="AB1" s="107"/>
-      <c r="AC1" s="107"/>
-      <c r="AD1" s="107"/>
-      <c r="AE1" s="107"/>
-      <c r="AF1" s="107"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="87"/>
+      <c r="R1" s="87"/>
+      <c r="S1" s="87"/>
+      <c r="T1" s="87"/>
+      <c r="U1" s="87"/>
+      <c r="V1" s="87"/>
+      <c r="W1" s="87"/>
+      <c r="X1" s="87"/>
+      <c r="Y1" s="87"/>
+      <c r="Z1" s="87"/>
+      <c r="AA1" s="87"/>
+      <c r="AB1" s="87"/>
+      <c r="AC1" s="87"/>
+      <c r="AD1" s="87"/>
+      <c r="AE1" s="87"/>
+      <c r="AF1" s="87"/>
     </row>
     <row r="2" spans="1:32" ht="15" customHeight="1">
       <c r="A2" s="114" t="s">
@@ -3079,18 +3094,18 @@
       <c r="S2" s="121"/>
       <c r="T2" s="121"/>
       <c r="U2" s="122"/>
-      <c r="W2" s="108" t="s">
+      <c r="W2" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="X2" s="109"/>
-      <c r="Y2" s="109"/>
-      <c r="Z2" s="109"/>
-      <c r="AA2" s="109"/>
-      <c r="AB2" s="109"/>
-      <c r="AC2" s="109"/>
-      <c r="AD2" s="109"/>
-      <c r="AE2" s="109"/>
-      <c r="AF2" s="110"/>
+      <c r="X2" s="89"/>
+      <c r="Y2" s="89"/>
+      <c r="Z2" s="89"/>
+      <c r="AA2" s="89"/>
+      <c r="AB2" s="89"/>
+      <c r="AC2" s="89"/>
+      <c r="AD2" s="89"/>
+      <c r="AE2" s="89"/>
+      <c r="AF2" s="90"/>
     </row>
     <row r="3" spans="1:32" ht="19.350000000000001" customHeight="1" thickBot="1">
       <c r="A3" s="117"/>
@@ -3113,16 +3128,16 @@
       <c r="S3" s="124"/>
       <c r="T3" s="124"/>
       <c r="U3" s="125"/>
-      <c r="W3" s="111"/>
-      <c r="X3" s="112"/>
-      <c r="Y3" s="112"/>
-      <c r="Z3" s="112"/>
-      <c r="AA3" s="112"/>
-      <c r="AB3" s="112"/>
-      <c r="AC3" s="112"/>
-      <c r="AD3" s="112"/>
-      <c r="AE3" s="112"/>
-      <c r="AF3" s="113"/>
+      <c r="W3" s="91"/>
+      <c r="X3" s="92"/>
+      <c r="Y3" s="92"/>
+      <c r="Z3" s="92"/>
+      <c r="AA3" s="92"/>
+      <c r="AB3" s="92"/>
+      <c r="AC3" s="92"/>
+      <c r="AD3" s="92"/>
+      <c r="AE3" s="92"/>
+      <c r="AF3" s="93"/>
     </row>
     <row r="4" spans="1:32" ht="18" customHeight="1">
       <c r="A4" s="94" t="s">
@@ -3137,10 +3152,10 @@
         <v>1</v>
       </c>
       <c r="H4" s="101"/>
-      <c r="I4" s="86" t="s">
+      <c r="I4" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="87"/>
+      <c r="J4" s="107"/>
       <c r="L4" s="94" t="s">
         <v>2</v>
       </c>
@@ -3153,10 +3168,10 @@
         <v>1</v>
       </c>
       <c r="S4" s="101"/>
-      <c r="T4" s="86" t="s">
+      <c r="T4" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="U4" s="87"/>
+      <c r="U4" s="107"/>
       <c r="W4" s="94" t="s">
         <v>2</v>
       </c>
@@ -3169,10 +3184,10 @@
         <v>1</v>
       </c>
       <c r="AD4" s="101"/>
-      <c r="AE4" s="86" t="s">
+      <c r="AE4" s="106" t="s">
         <v>3</v>
       </c>
-      <c r="AF4" s="87"/>
+      <c r="AF4" s="107"/>
     </row>
     <row r="5" spans="1:32" ht="15.75" thickBot="1">
       <c r="A5" s="97"/>
@@ -3183,8 +3198,8 @@
       <c r="F5" s="99"/>
       <c r="G5" s="102"/>
       <c r="H5" s="103"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="89"/>
+      <c r="I5" s="108"/>
+      <c r="J5" s="109"/>
       <c r="L5" s="97"/>
       <c r="M5" s="98"/>
       <c r="N5" s="98"/>
@@ -3193,8 +3208,8 @@
       <c r="Q5" s="127"/>
       <c r="R5" s="102"/>
       <c r="S5" s="103"/>
-      <c r="T5" s="88"/>
-      <c r="U5" s="89"/>
+      <c r="T5" s="108"/>
+      <c r="U5" s="109"/>
       <c r="W5" s="97"/>
       <c r="X5" s="98"/>
       <c r="Y5" s="98"/>
@@ -3203,30 +3218,30 @@
       <c r="AB5" s="99"/>
       <c r="AC5" s="102"/>
       <c r="AD5" s="103"/>
-      <c r="AE5" s="88"/>
-      <c r="AF5" s="89"/>
+      <c r="AE5" s="108"/>
+      <c r="AF5" s="109"/>
     </row>
     <row r="6" spans="1:32" ht="15.75" thickBot="1">
-      <c r="A6" s="92" t="s">
+      <c r="A6" s="112" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="93"/>
-      <c r="C6" s="92" t="s">
+      <c r="B6" s="113"/>
+      <c r="C6" s="112" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="93"/>
-      <c r="E6" s="92" t="s">
+      <c r="D6" s="113"/>
+      <c r="E6" s="112" t="s">
         <v>101</v>
       </c>
-      <c r="F6" s="93"/>
+      <c r="F6" s="113"/>
       <c r="G6" s="104"/>
       <c r="H6" s="105"/>
-      <c r="I6" s="90"/>
-      <c r="J6" s="91"/>
-      <c r="L6" s="92" t="s">
+      <c r="I6" s="110"/>
+      <c r="J6" s="111"/>
+      <c r="L6" s="112" t="s">
         <v>99</v>
       </c>
-      <c r="M6" s="93"/>
+      <c r="M6" s="113"/>
       <c r="N6" s="128" t="s">
         <v>100</v>
       </c>
@@ -3237,24 +3252,24 @@
       <c r="Q6" s="130"/>
       <c r="R6" s="104"/>
       <c r="S6" s="105"/>
-      <c r="T6" s="90"/>
-      <c r="U6" s="91"/>
-      <c r="W6" s="92" t="s">
+      <c r="T6" s="110"/>
+      <c r="U6" s="111"/>
+      <c r="W6" s="112" t="s">
         <v>99</v>
       </c>
-      <c r="X6" s="93"/>
-      <c r="Y6" s="92" t="s">
+      <c r="X6" s="113"/>
+      <c r="Y6" s="112" t="s">
         <v>100</v>
       </c>
-      <c r="Z6" s="93"/>
-      <c r="AA6" s="92" t="s">
+      <c r="Z6" s="113"/>
+      <c r="AA6" s="112" t="s">
         <v>101</v>
       </c>
-      <c r="AB6" s="93"/>
+      <c r="AB6" s="113"/>
       <c r="AC6" s="104"/>
       <c r="AD6" s="105"/>
-      <c r="AE6" s="90"/>
-      <c r="AF6" s="91"/>
+      <c r="AE6" s="110"/>
+      <c r="AF6" s="111"/>
     </row>
     <row r="7" spans="1:32" ht="15.75" thickBot="1">
       <c r="A7" s="25" t="s">
@@ -3679,8 +3694,12 @@
       <c r="O12" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="P12" s="10"/>
-      <c r="Q12" s="28"/>
+      <c r="P12" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q12" s="28" t="s">
+        <v>189</v>
+      </c>
       <c r="R12" s="10"/>
       <c r="S12" s="6"/>
       <c r="T12" s="10"/>
@@ -3696,7 +3715,7 @@
       <c r="AE12" s="10"/>
       <c r="AF12" s="6"/>
     </row>
-    <row r="13" spans="1:32">
+    <row r="13" spans="1:32" ht="30">
       <c r="A13" s="10" t="s">
         <v>107</v>
       </c>
@@ -3731,8 +3750,12 @@
       <c r="O13" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="28"/>
+      <c r="P13" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q13" s="28" t="s">
+        <v>191</v>
+      </c>
       <c r="R13" s="10"/>
       <c r="S13" s="6"/>
       <c r="T13" s="10"/>
@@ -3779,8 +3802,12 @@
       <c r="O14" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="28"/>
+      <c r="P14" s="10" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q14" s="28" t="s">
+        <v>62</v>
+      </c>
       <c r="R14" s="10"/>
       <c r="S14" s="6"/>
       <c r="T14" s="10"/>
@@ -3858,6 +3885,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="I4:J6"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="A4:F5"/>
+    <mergeCell ref="G4:H6"/>
     <mergeCell ref="A1:AF1"/>
     <mergeCell ref="W2:AF3"/>
     <mergeCell ref="W4:AB5"/>
@@ -3874,12 +3907,6 @@
     <mergeCell ref="L6:M6"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="I4:J6"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="A4:F5"/>
-    <mergeCell ref="G4:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>